<commit_message>
fixing mongo issue and adding burn down chart updates
</commit_message>
<xml_diff>
--- a/burndown-chart-journal/Fantastic-4-Burndown-Chart-July-17.xlsx
+++ b/burndown-chart-journal/Fantastic-4-Burndown-Chart-July-17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SJSU\GIT\su18-202-fantastic-4\burndown-chart-journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D306C92-678A-4455-9F83-798067832E89}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF80BB8-7FC6-4129-9988-3E1AF1B60B36}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,12 +174,14 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -187,6 +189,7 @@
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -198,16 +201,19 @@
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -512,16 +518,22 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -529,12 +541,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +779,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -887,7 +893,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,7 +1378,7 @@
   <dimension ref="A1:Q999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1389,34 +1395,34 @@
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="46" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="42"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1457,10 +1463,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="45"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="7">
         <v>43297</v>
       </c>
@@ -1500,9 +1506,9 @@
       <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="24" customHeight="1">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10">
         <v>40</v>
@@ -1555,9 +1561,9 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="24" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="15">
         <v>40</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="12">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G5" s="12">
         <v>4</v>
@@ -1619,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="22">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -1633,7 +1639,7 @@
       <c r="P6" s="25"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="45" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -1659,7 +1665,7 @@
       <c r="P7" s="25"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A8" s="38"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="18" t="s">
         <v>25</v>
       </c>
@@ -1687,7 +1693,7 @@
       <c r="P8" s="25"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A9" s="38"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="18" t="s">
         <v>27</v>
       </c>
@@ -1715,7 +1721,7 @@
       <c r="P9" s="25"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A10" s="38"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="18" t="s">
         <v>29</v>
       </c>
@@ -1743,7 +1749,7 @@
       <c r="P10" s="25"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A11" s="38"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="18" t="s">
         <v>31</v>
       </c>
@@ -1765,7 +1771,7 @@
       <c r="P11" s="25"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A12" s="38"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="18" t="s">
         <v>32</v>
       </c>
@@ -1787,7 +1793,7 @@
       <c r="P12" s="25"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A13" s="39"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="18" t="s">
         <v>33</v>
       </c>
@@ -1831,7 +1837,7 @@
       <c r="P14" s="25"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="40" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="18" t="s">
@@ -1853,7 +1859,7 @@
       <c r="P15" s="25"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A16" s="39"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="29" t="s">
         <v>37</v>
       </c>

</xml_diff>